<commit_message>
OneR, ID3 and C45 data added
</commit_message>
<xml_diff>
--- a/Coursework 2/courseworkData/Clean Data.xlsx
+++ b/Coursework 2/courseworkData/Clean Data.xlsx
@@ -44,121 +44,121 @@
     <t>Decision</t>
   </si>
   <si>
-    <t>0&lt;=X&lt;200</t>
+    <t>'0&lt;=X&lt;200'</t>
   </si>
   <si>
-    <t>existing paid</t>
+    <t>'existing paid'</t>
   </si>
   <si>
-    <t>radio/tv</t>
+    <t>'radio/tv'</t>
   </si>
   <si>
-    <t>&lt;100</t>
+    <t>'&lt;100'</t>
   </si>
   <si>
-    <t>1&lt;=X&lt;4</t>
+    <t>'1&lt;=X&lt;4'</t>
   </si>
   <si>
-    <t>female div/dep/mar</t>
+    <t>'female div/dep/mar'</t>
   </si>
   <si>
-    <t>skilled</t>
+    <t>'skilled'</t>
   </si>
   <si>
     <t>bad</t>
   </si>
   <si>
-    <t>no checking</t>
+    <t>'no checking'</t>
   </si>
   <si>
-    <t>critical/other existing credit</t>
+    <t>'critical/other existing credit'</t>
   </si>
   <si>
-    <t>education</t>
+    <t>'education'</t>
   </si>
   <si>
-    <t>4&lt;=X&lt;7</t>
+    <t>'4&lt;=X&lt;7'</t>
   </si>
   <si>
-    <t>male single</t>
+    <t>'male single'</t>
   </si>
   <si>
-    <t>unskilled resident</t>
+    <t>'unskilled resident'</t>
   </si>
   <si>
     <t>good</t>
   </si>
   <si>
-    <t>&lt;0</t>
+    <t>'&lt;0'</t>
   </si>
   <si>
-    <t>furniture/equipment</t>
+    <t>'furniture/equipment'</t>
   </si>
   <si>
-    <t>delayed previously</t>
+    <t>'delayed previously'</t>
   </si>
   <si>
-    <t>new car</t>
+    <t>'new car'</t>
   </si>
   <si>
-    <t>no known savings</t>
+    <t>'no known savings'</t>
   </si>
   <si>
-    <t>500&lt;=X&lt;1000</t>
+    <t>'500&lt;=X&lt;1000'</t>
   </si>
   <si>
-    <t>&gt;=7</t>
+    <t>'&gt;=7'</t>
   </si>
   <si>
-    <t>used car</t>
+    <t>'used car'</t>
   </si>
   <si>
-    <t>high qualif/self emp/mgmt</t>
+    <t>'high qualif/self emp/mgmt'</t>
   </si>
   <si>
-    <t>&gt;=1000</t>
+    <t>'&gt;=1000'</t>
   </si>
   <si>
-    <t>male div/sep</t>
+    <t>'male div/sep'</t>
   </si>
   <si>
-    <t>unemployed</t>
+    <t>'unemployed'</t>
   </si>
   <si>
-    <t>male mar/wid</t>
+    <t>'male mar/wid'</t>
   </si>
   <si>
-    <t>&lt;1</t>
+    <t>'&lt;1'</t>
   </si>
   <si>
-    <t>business</t>
+    <t>'business'</t>
   </si>
   <si>
-    <t>100&lt;=X&lt;500</t>
+    <t>'100&lt;=X&lt;500'</t>
   </si>
   <si>
-    <t>no credits/all paid</t>
+    <t>'no credits/all paid'</t>
   </si>
   <si>
-    <t>&gt;=200</t>
+    <t>'&gt;=200'</t>
   </si>
   <si>
-    <t>all paid</t>
+    <t>'all paid'</t>
   </si>
   <si>
-    <t>domestic appliance</t>
+    <t>'domestic appliance'</t>
   </si>
   <si>
-    <t>repairs</t>
+    <t>'repairs'</t>
   </si>
   <si>
-    <t>unemp/unskilled non res</t>
+    <t>'unemp/unskilled non res'</t>
   </si>
   <si>
-    <t>other</t>
+    <t>'other'</t>
   </si>
   <si>
-    <t>retraining</t>
+    <t>'retraining'</t>
   </si>
 </sst>
 </file>

</xml_diff>